<commit_message>
Import XLSX file added
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Dave</t>
   </si>
@@ -46,6 +46,30 @@
   </si>
   <si>
     <t>bla@testtest.nl</t>
+  </si>
+  <si>
+    <t>Dennis</t>
+  </si>
+  <si>
+    <t>den@nis.nis</t>
+  </si>
+  <si>
+    <t>Cooker</t>
+  </si>
+  <si>
+    <t>cook@er.errr</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>tester@test.se</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>jacklo@ers.se</t>
   </si>
 </sst>
 </file>
@@ -105,15 +129,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -391,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,12 +473,60 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B3" r:id="rId3"/>
     <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
+    <hyperlink ref="B7" r:id="rId7"/>
+    <hyperlink ref="B8" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>